<commit_message>
All series numbers in all transactions will reset every year
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kervic\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\purchasing\uploads\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39CCAF2-04F7-4CDC-9008-B686E37A4280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
+  <si>
+    <t>Central Negros Power Reliability, Inc.</t>
+  </si>
   <si>
     <t>(Main Office) 88 Corner Rizal-Mabini Sts. Bacolod City</t>
   </si>
@@ -219,47 +223,19 @@
     <t>Requested By:</t>
   </si>
   <si>
+    <t>GENERAL DESCRIPTION</t>
+  </si>
+  <si>
     <t>YYYY-MM-DD</t>
   </si>
   <si>
-    <t xml:space="preserve"> PROGEN DIESELTECH SERVICES CORP.</t>
-  </si>
-  <si>
-    <t>PROGEN</t>
-  </si>
-  <si>
-    <t>PROJO-BCD22-008</t>
-  </si>
-  <si>
-    <t>IPRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fabrication of Valve Seat Ring Insert Puller Parts for Sulzer Cylinder Head </t>
-  </si>
-  <si>
-    <t>Gino M. Lovico</t>
-  </si>
-  <si>
-    <t>Supply of Labor, Material, Tools &amp; Equipment and Technical Expertise</t>
-  </si>
-  <si>
-    <t>Mr. Lovico will supervise and monitor the fabrication.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fabrication of Sulzer Cylinder Head Valve Seat Ring Insert Puller Parts
-1. Clamping Jaws - 4pcs
-2. Cones - 1set
-Materials: SAE 4140
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lot </t>
+    <t>REFER TO DEPARTMENT CODE SHEET</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
@@ -477,103 +453,103 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -602,26 +578,32 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>50273</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>140387</xdr:rowOff>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -634,8 +616,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="695325" y="240773"/>
-          <a:ext cx="571500" cy="671139"/>
+          <a:off x="19050" y="381000"/>
+          <a:ext cx="1200150" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -909,11 +891,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="C9" sqref="C9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,14 +925,14 @@
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="C2" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="5"/>
@@ -958,14 +940,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
+      <c r="C3" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -973,14 +955,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
+      <c r="C4" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -988,255 +970,297 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
+      <c r="C5" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="26"/>
+      <c r="A6" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="43"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="21"/>
+      <c r="A7" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="21"/>
+        <v>55</v>
+      </c>
+      <c r="I7" s="25"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="27"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="31">
-        <v>44628</v>
-      </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="36"/>
+      <c r="A8" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="36"/>
+      <c r="C8" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" s="32"/>
-      <c r="K8" s="33"/>
+        <v>58</v>
+      </c>
+      <c r="I8" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="46"/>
+      <c r="K8" s="47"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
+      <c r="A9" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="24"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="J9" s="35"/>
-      <c r="K9" s="36"/>
+        <v>59</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="23"/>
+      <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="21"/>
+      <c r="A10" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="27"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" s="20">
-        <v>1</v>
-      </c>
-      <c r="J10" s="34"/>
-      <c r="K10" s="21"/>
+        <v>9</v>
+      </c>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="27"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="21"/>
+      <c r="A11" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="31"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="49"/>
+        <v>8</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="39"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J13" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="K13" s="40"/>
+      <c r="K13" s="29"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="46"/>
-    </row>
-    <row r="15" spans="1:11" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
-        <v>1</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>73</v>
-      </c>
+      <c r="A14" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="35"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
-      <c r="G15" s="14">
-        <v>1</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>74</v>
-      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="13"/>
       <c r="I15" s="13"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="38"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>72</v>
-      </c>
+      <c r="A16" s="13"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="21"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="20"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="21"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="20"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="17"/>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="21"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="27"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="27"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="37">
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="A10:B10"/>
@@ -1251,23 +1275,6 @@
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="C12:K12"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="J16:K16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="360" r:id="rId1"/>
@@ -1276,7 +1283,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1290,178 +1297,178 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
export and import upgrade to php8
</commit_message>
<xml_diff>
--- a/uploads/excel/JORequestForm.xlsx
+++ b/uploads/excel/JORequestForm.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\purchasing\uploads\format\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Glenn\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39CCAF2-04F7-4CDC-9008-B686E37A4280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
-  <si>
-    <t>Central Negros Power Reliability, Inc.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>(Main Office) 88 Corner Rizal-Mabini Sts. Bacolod City</t>
   </si>
@@ -226,16 +222,28 @@
     <t>GENERAL DESCRIPTION</t>
   </si>
   <si>
-    <t>YYYY-MM-DD</t>
-  </si>
-  <si>
-    <t>REFER TO DEPARTMENT CODE SHEET</t>
+    <t xml:space="preserve"> PROGEN DIESELTECH SERVICES CORP.</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>pcs</t>
+  </si>
+  <si>
+    <t>sss</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>www</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
@@ -424,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -537,12 +545,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -578,32 +580,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>50273</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>140387</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -616,8 +612,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19050" y="381000"/>
-          <a:ext cx="1200150" cy="304800"/>
+          <a:off x="695325" y="240773"/>
+          <a:ext cx="571500" cy="671139"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -891,11 +887,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,7 +922,7 @@
       <c r="A2" s="3"/>
       <c r="B2" s="10"/>
       <c r="C2" s="44" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="D2" s="44"/>
       <c r="E2" s="44"/>
@@ -941,7 +937,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="45"/>
       <c r="E3" s="45"/>
@@ -956,7 +952,7 @@
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="45" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="45"/>
       <c r="E4" s="45"/>
@@ -971,7 +967,7 @@
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="40"/>
       <c r="E5" s="40"/>
@@ -984,7 +980,7 @@
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="42"/>
       <c r="C6" s="42"/>
@@ -999,7 +995,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="25"/>
@@ -1008,7 +1004,7 @@
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I7" s="25"/>
       <c r="J7" s="26"/>
@@ -1016,49 +1012,49 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="36"/>
-      <c r="C8" s="22" t="s">
-        <v>66</v>
+      <c r="C8" s="22">
+        <v>45176</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="24"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="I8" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="J8" s="46"/>
-      <c r="K8" s="47"/>
+        <v>57</v>
+      </c>
+      <c r="I8" s="22">
+        <v>45176</v>
+      </c>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="36"/>
       <c r="C9" s="22" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="24"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="22" t="s">
-        <v>66</v>
+        <v>58</v>
+      </c>
+      <c r="I9" s="22">
+        <v>45176</v>
       </c>
       <c r="J9" s="23"/>
       <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="25"/>
@@ -1067,7 +1063,7 @@
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I10" s="25"/>
       <c r="J10" s="26"/>
@@ -1075,7 +1071,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="31"/>
       <c r="C11" s="25"/>
@@ -1091,7 +1087,7 @@
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="37"/>
       <c r="D12" s="38"/>
@@ -1105,32 +1101,32 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
       <c r="F13" s="29"/>
       <c r="G13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="I13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" s="28" t="s">
         <v>60</v>
-      </c>
-      <c r="J13" s="28" t="s">
-        <v>61</v>
       </c>
       <c r="K13" s="29"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="34"/>
       <c r="C14" s="34"/>
@@ -1144,16 +1140,28 @@
       <c r="K14" s="35"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="17"/>
+      <c r="A15" s="13">
+        <v>1</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>66</v>
+      </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="19"/>
+      <c r="G15" s="14">
+        <v>1</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="13">
+        <v>100</v>
+      </c>
+      <c r="J15" s="19">
+        <v>100</v>
+      </c>
       <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1197,13 +1205,15 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="17"/>
+        <v>62</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>68</v>
+      </c>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="49"/>
+      <c r="F19" s="47"/>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
@@ -1212,11 +1222,13 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
-      <c r="B20" s="48"/>
+      <c r="B20" s="46" t="s">
+        <v>69</v>
+      </c>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="49"/>
+      <c r="F20" s="47"/>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
@@ -1225,11 +1237,13 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
-      <c r="B21" s="48"/>
+      <c r="B21" s="46" t="s">
+        <v>70</v>
+      </c>
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="49"/>
+      <c r="F21" s="47"/>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
       <c r="I21" s="16"/>
@@ -1283,7 +1297,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1297,178 +1311,178 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
         <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
         <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
         <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
         <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
         <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
         <v>39</v>
-      </c>
-      <c r="B16" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
         <v>41</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
         <v>43</v>
-      </c>
-      <c r="B18" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
         <v>45</v>
-      </c>
-      <c r="B19" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
         <v>47</v>
-      </c>
-      <c r="B20" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
         <v>49</v>
-      </c>
-      <c r="B21" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
         <v>51</v>
-      </c>
-      <c r="B22" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>